<commit_message>
Fixed dipoles, and bug with segmentation
</commit_message>
<xml_diff>
--- a/Beamline_elements.xlsx
+++ b/Beamline_elements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NielsB\cernbox\Hawaii University\Beam dynamics\FEL_sim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NielsB\cernbox\Hawaii University\Beam dynamics\FELsim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED83790-314D-4F57-885D-AABA909798F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FAFAE6F-3F0E-4A97-B48C-E0629B98CFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3612" yWindow="300" windowWidth="25944" windowHeight="15372" xr2:uid="{4C82D9F0-9D94-4EC2-AD9E-40D58C931DEF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="34776" windowHeight="21096" xr2:uid="{4C82D9F0-9D94-4EC2-AD9E-40D58C931DEF}"/>
   </bookViews>
   <sheets>
     <sheet name="pysheet_" sheetId="2" r:id="rId1"/>
@@ -1814,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033554DD-3897-4359-B7DF-3FC088E3C719}">
   <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="N62" sqref="N62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2241,7 +2241,7 @@
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="str">
         <f>M14 &amp; "."  &amp; N14 &amp; "." &amp; TEXT(10*IF(ISNUMBER(C14), C14, F14), "000")</f>
-        <v>DC1.QPC.021</v>
+        <v>DC1.QPF.021</v>
       </c>
       <c r="B14" s="16">
         <f>D12+Sheet1!B7</f>
@@ -2272,7 +2272,7 @@
         <v>250</v>
       </c>
       <c r="N14" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -2416,7 +2416,7 @@
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="str">
         <f>M19 &amp; "."  &amp; N19 &amp; "." &amp; TEXT(10*IF(ISNUMBER(C19), C19, F19), "000")</f>
-        <v>DC2.QPF.028</v>
+        <v>DC2.QPD.028</v>
       </c>
       <c r="B19" s="16">
         <f>D16+Sheet1!B9</f>
@@ -2447,13 +2447,13 @@
         <v>251</v>
       </c>
       <c r="N19" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="str">
         <f>M20 &amp; "."  &amp; N20 &amp; "." &amp; TEXT(10*IF(ISNUMBER(C20), C20, F20), "000")</f>
-        <v>DC2.QPD.029</v>
+        <v>DC2.QPF.029</v>
       </c>
       <c r="B20" s="16">
         <f>D19+Sheet1!B10</f>
@@ -2484,13 +2484,13 @@
         <v>251</v>
       </c>
       <c r="N20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="str">
         <f>M21 &amp; "."  &amp; N21 &amp; "." &amp; TEXT(10*IF(ISNUMBER(C21), C21, F21), "000")</f>
-        <v>DC2.QPF.030</v>
+        <v>DC2.QPD.030</v>
       </c>
       <c r="B21" s="16">
         <f>D20+Sheet1!B11</f>
@@ -2521,7 +2521,7 @@
         <v>251</v>
       </c>
       <c r="N21" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -2574,7 +2574,7 @@
         <v>3.2979100000000008</v>
       </c>
       <c r="F23" s="20">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="G23">
         <v>4.0640000000000003E-2</v>
@@ -2610,7 +2610,7 @@
         <v>3.3385500000000006</v>
       </c>
       <c r="F24" s="20">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="G24">
         <v>4.0640000000000003E-2</v>
@@ -2649,7 +2649,7 @@
         <v>3.3485500000000004</v>
       </c>
       <c r="F25" s="20">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="G25">
         <v>4.0640000000000003E-2</v>
@@ -2670,7 +2670,7 @@
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>DC2.QPC.036</v>
+        <v>DC2.QPF.036</v>
       </c>
       <c r="B26" s="16">
         <f>D24+Sheet1!B14</f>
@@ -2701,7 +2701,7 @@
         <v>251</v>
       </c>
       <c r="N26" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
@@ -2722,7 +2722,7 @@
         <v>3.8593100000000011</v>
       </c>
       <c r="F27" s="20">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="G27">
         <v>4.0640000000000003E-2</v>
@@ -2758,7 +2758,7 @@
         <v>3.8999500000000009</v>
       </c>
       <c r="F28" s="20">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="G28">
         <v>4.0640000000000003E-2</v>
@@ -2797,7 +2797,7 @@
         <v>3.9099500000000007</v>
       </c>
       <c r="F29" s="20">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="G29">
         <v>4.0640000000000003E-2</v>
@@ -2886,7 +2886,7 @@
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="str">
         <f>M32 &amp; "."  &amp; N32 &amp; "." &amp; TEXT(10*IF(ISNUMBER(C32), C32, F32), "000")</f>
-        <v>DC2.QPF.042</v>
+        <v>DC2.QPD.042</v>
       </c>
       <c r="B32" s="16">
         <f>D28+Sheet1!B16</f>
@@ -2917,13 +2917,13 @@
         <v>251</v>
       </c>
       <c r="N32" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="str">
         <f>M33 &amp; "."  &amp; N33 &amp; "." &amp; TEXT(10*IF(ISNUMBER(C33), C33, F33), "000")</f>
-        <v>DC2.QPD.043</v>
+        <v>DC2.QPF.043</v>
       </c>
       <c r="B33" s="16">
         <f>D32+Sheet1!B17</f>
@@ -2954,13 +2954,13 @@
         <v>251</v>
       </c>
       <c r="N33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="str">
         <f>M34 &amp; "."  &amp; N34 &amp; "." &amp; TEXT(10*IF(ISNUMBER(C34), C34, F34), "000")</f>
-        <v>DC2.QPF.045</v>
+        <v>DC2.QPD.045</v>
       </c>
       <c r="B34" s="16">
         <f>D33+Sheet1!B18</f>
@@ -2991,7 +2991,7 @@
         <v>251</v>
       </c>
       <c r="N34" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
@@ -3026,7 +3026,7 @@
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="str">
         <f>M36 &amp; "."  &amp; N36 &amp; "." &amp; TEXT(10*IF(ISNUMBER(C36), C36, F36), "000")</f>
-        <v>DC3.QPF.050</v>
+        <v>DC3.QPD.050</v>
       </c>
       <c r="B36" s="16">
         <f>D34+Sheet1!B19</f>
@@ -3057,13 +3057,13 @@
         <v>252</v>
       </c>
       <c r="N36" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="str">
         <f>M37 &amp; "."  &amp; N37 &amp; "." &amp; TEXT(10*IF(ISNUMBER(C37), C37, F37), "000")</f>
-        <v>DC3.QPD.051</v>
+        <v>DC3.QPF.051</v>
       </c>
       <c r="B37" s="16">
         <f>D36+Sheet1!B20</f>
@@ -3094,13 +3094,13 @@
         <v>252</v>
       </c>
       <c r="N37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="str">
         <f>M38 &amp; "."  &amp; N38 &amp; "." &amp; TEXT(10*IF(ISNUMBER(C38), C38, F38), "000")</f>
-        <v>DC3.QPF.053</v>
+        <v>DC3.QPD.053</v>
       </c>
       <c r="B38" s="16">
         <f>D37+Sheet1!B21</f>
@@ -3131,7 +3131,7 @@
         <v>252</v>
       </c>
       <c r="N38" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
@@ -3301,7 +3301,7 @@
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="str">
         <f>M44 &amp; "."  &amp; N44 &amp; "." &amp; TEXT(10*IF(ISNUMBER(C44), C44, F44), "000")</f>
-        <v>DC3.QPC.059</v>
+        <v>DC3.QPF.059</v>
       </c>
       <c r="B44" s="16">
         <f>D41+Sheet1!B24</f>
@@ -3332,7 +3332,7 @@
         <v>252</v>
       </c>
       <c r="N44" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
@@ -3538,7 +3538,7 @@
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="str">
         <f>M51 &amp; "."  &amp; N51 &amp; "." &amp; TEXT(10*IF(ISNUMBER(C51), C51, F51), "000")</f>
-        <v>DC3.QPF.064</v>
+        <v>DC3.QPD.064</v>
       </c>
       <c r="B51" s="16">
         <f>D47+Sheet1!B26</f>
@@ -3569,13 +3569,13 @@
         <v>252</v>
       </c>
       <c r="N51" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="str">
         <f>M52 &amp; "."  &amp; N52 &amp; "." &amp; TEXT(10*IF(ISNUMBER(C52), C52, F52), "000")</f>
-        <v>DC3.QPD.066</v>
+        <v>DC3.QPF.066</v>
       </c>
       <c r="B52" s="16">
         <f>D51+Sheet1!B27</f>
@@ -3606,7 +3606,7 @@
         <v>252</v>
       </c>
       <c r="N52" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.3">
@@ -3832,7 +3832,7 @@
         <v>7.4145199999999969</v>
       </c>
       <c r="E60">
-        <v>2.2557535263548631</v>
+        <v>2.4870081662954718E-2</v>
       </c>
       <c r="F60" s="20"/>
       <c r="J60" s="7" t="s">
@@ -3869,7 +3869,7 @@
         <v>7.5588199999999963</v>
       </c>
       <c r="E61">
-        <v>1.6718634001484785</v>
+        <v>1E-3</v>
       </c>
       <c r="F61" s="20"/>
       <c r="J61" s="19" t="s">
@@ -3938,7 +3938,7 @@
         <v>7.8509199999999959</v>
       </c>
       <c r="F63" s="20">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="G63">
         <v>4.0640000000000003E-2</v>
@@ -3974,7 +3974,7 @@
         <v>7.8915599999999957</v>
       </c>
       <c r="F64" s="20">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="G64">
         <v>4.0640000000000003E-2</v>
@@ -4013,7 +4013,7 @@
         <v>7.9015599999999955</v>
       </c>
       <c r="F65" s="20">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="G65">
         <v>4.0640000000000003E-2</v>
@@ -4070,7 +4070,7 @@
         <v>8.1963899999999956</v>
       </c>
       <c r="E67">
-        <v>2.7097253155159615</v>
+        <v>4.4914625092798817</v>
       </c>
       <c r="F67" s="20"/>
       <c r="J67" s="7" t="s">
@@ -4086,7 +4086,7 @@
         <v>253</v>
       </c>
       <c r="N67" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.3">
@@ -4125,7 +4125,7 @@
         <v>8.4123199999999958</v>
       </c>
       <c r="F69" s="20">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="G69">
         <v>4.0640000000000003E-2</v>
@@ -4161,7 +4161,7 @@
         <v>8.4529599999999956</v>
       </c>
       <c r="F70" s="20">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="G70">
         <v>4.0640000000000003E-2</v>
@@ -4200,7 +4200,7 @@
         <v>8.4629599999999954</v>
       </c>
       <c r="F71" s="20">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="G71">
         <v>4.0640000000000003E-2</v>
@@ -4252,7 +4252,7 @@
         <v>253</v>
       </c>
       <c r="N72" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">
@@ -4289,7 +4289,7 @@
         <v>253</v>
       </c>
       <c r="N73" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.3">
@@ -4326,7 +4326,7 @@
         <v>253</v>
       </c>
       <c r="N74" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.3">
@@ -4596,7 +4596,7 @@
         <v>9.7177929999999968</v>
       </c>
       <c r="E83">
-        <v>0.77691165553080932</v>
+        <v>3.8166035634743878</v>
       </c>
       <c r="F83" s="20"/>
       <c r="J83" s="7" t="s">
@@ -4610,7 +4610,7 @@
         <v>254</v>
       </c>
       <c r="N83" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.3">
@@ -4781,7 +4781,7 @@
         <v>254</v>
       </c>
       <c r="N88" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.3">
@@ -4964,13 +4964,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC6263B-129C-4012-8C81-A56CA3901853}">
   <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8095,7 +8096,7 @@
   <dimension ref="A1:S58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9810,7 +9811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C826FC-82B6-4AF9-95D8-27CD617DC0AA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB33" sqref="AB33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed dipoles, dispersion / testing optimization on UH line
</commit_message>
<xml_diff>
--- a/Beamline_elements.xlsx
+++ b/Beamline_elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NielsB\cernbox\Hawaii University\Beam dynamics\FELsim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FAFAE6F-3F0E-4A97-B48C-E0629B98CFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF57E20-CD6D-439F-AD44-8A8E64D9DC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="34776" windowHeight="21096" xr2:uid="{4C82D9F0-9D94-4EC2-AD9E-40D58C931DEF}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="25920" windowHeight="15360" xr2:uid="{4C82D9F0-9D94-4EC2-AD9E-40D58C931DEF}"/>
   </bookViews>
   <sheets>
     <sheet name="pysheet_" sheetId="2" r:id="rId1"/>
@@ -1814,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033554DD-3897-4359-B7DF-3FC088E3C719}">
   <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="N62" sqref="N62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1910,7 +1910,7 @@
         <v>0.44767500000000005</v>
       </c>
       <c r="E3">
-        <v>0.91685226429101718</v>
+        <v>0.88571930929915599</v>
       </c>
       <c r="F3" s="20"/>
       <c r="J3" s="7" t="s">
@@ -1967,7 +1967,7 @@
         <v>0.73342499999999999</v>
       </c>
       <c r="E5">
-        <v>1.0764662212323683</v>
+        <v>1.0528901226284999</v>
       </c>
       <c r="F5" s="20"/>
       <c r="J5" s="7" t="s">
@@ -8095,8 +8095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690C5098-DD13-4632-A393-CDBA5D4508EB}">
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fix on wedge dipole
</commit_message>
<xml_diff>
--- a/Beamline_elements.xlsx
+++ b/Beamline_elements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NielsB\cernbox\Hawaii University\Beam dynamics\FELsim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF57E20-CD6D-439F-AD44-8A8E64D9DC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671CB04F-7346-4577-A427-C5BBE5067470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="2616" windowWidth="25920" windowHeight="15360" xr2:uid="{4C82D9F0-9D94-4EC2-AD9E-40D58C931DEF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="34776" windowHeight="21096" xr2:uid="{4C82D9F0-9D94-4EC2-AD9E-40D58C931DEF}"/>
   </bookViews>
   <sheets>
     <sheet name="pysheet_" sheetId="2" r:id="rId1"/>
@@ -1814,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033554DD-3897-4359-B7DF-3FC088E3C719}">
   <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4964,8 +4964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC6263B-129C-4012-8C81-A56CA3901853}">
   <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
JupyterNotebook for beamline optimization
</commit_message>
<xml_diff>
--- a/Beamline_elements.xlsx
+++ b/Beamline_elements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NielsB\cernbox\Hawaii University\Beam dynamics\FELsim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671CB04F-7346-4577-A427-C5BBE5067470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F7FB9E-4F8A-4842-9B38-4310E7113E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="34776" windowHeight="21096" xr2:uid="{4C82D9F0-9D94-4EC2-AD9E-40D58C931DEF}"/>
   </bookViews>
@@ -1814,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033554DD-3897-4359-B7DF-3FC088E3C719}">
   <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="N89" sqref="N89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4781,7 +4781,7 @@
         <v>254</v>
       </c>
       <c r="N88" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.3">
@@ -4964,8 +4964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC6263B-129C-4012-8C81-A56CA3901853}">
   <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8096,7 +8096,7 @@
   <dimension ref="A1:S58"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>